<commit_message>
First pass at documentation
</commit_message>
<xml_diff>
--- a/inst/extdata/sleepIPD_metadata_template.xlsx
+++ b/inst/extdata/sleepIPD_metadata_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taren\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taren\GitHub\sleepIPD\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B393CD-D6A8-4CE7-9BDA-36A7D52431A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817C13BE-4D88-4A12-9CC9-D5206D1CA7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11895" yWindow="615" windowWidth="31365" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22350" yWindow="0" windowWidth="29370" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t xml:space="preserve">2-level scale </t>
   </si>
   <si>
-    <t>‘Better off’ or ‘poor’ based on basic needs being met (e.g. water, electricity).</t>
-  </si>
-  <si>
     <t>SIMD rank decile</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t xml:space="preserve">Mother education </t>
   </si>
   <si>
-    <t>1=10th grade or less, 2=vocational education, 3=high school education, 4=short tertiary education, 5=bachelor’s degree or equivalent, 6=master’s degree or higher.</t>
-  </si>
-  <si>
     <t>Parent education</t>
   </si>
   <si>
@@ -333,6 +327,12 @@
   </si>
   <si>
     <t>Ethnicity</t>
+  </si>
+  <si>
+    <t>Better off' or 'poor' based on basic needs being met (e.g. water, electricity).</t>
+  </si>
+  <si>
+    <t>1=10th grade or less, 2=vocational education, 3=high school education, 4=short tertiary education, 5=bachelor's degree or equivalent, 6=master's degree or higher.</t>
   </si>
 </sst>
 </file>
@@ -405,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -413,6 +413,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,10 +697,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -713,9 +714,9 @@
     <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -742,32 +743,29 @@
         <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -778,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5EF2728-2369-450A-B5D5-1F6C65BB68AD}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A1:A17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -791,10 +789,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -810,7 +808,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -858,77 +856,77 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -942,7 +940,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -962,8 +960,8 @@
       <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
-        <v>16</v>
+      <c r="D1" s="7" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -971,13 +969,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -985,13 +983,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -999,13 +997,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1013,13 +1011,13 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1027,13 +1025,13 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
         <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1041,13 +1039,13 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
         <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1055,13 +1053,13 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
         <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1069,13 +1067,13 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1083,7 +1081,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish vignette first draft
</commit_message>
<xml_diff>
--- a/inst/extdata/sleepIPD_metadata_template.xlsx
+++ b/inst/extdata/sleepIPD_metadata_template.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taren\GitHub\sleepIPD\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hartw\OneDrive\Desktop\ACU\RESEARCH\POOLED SLEEP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817C13BE-4D88-4A12-9CC9-D5206D1CA7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A857E8FD-74CB-4C39-92D4-E21FCD3D62E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22350" yWindow="0" windowWidth="29370" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Dictionary" sheetId="4" r:id="rId2"/>
     <sheet name="SES scales " sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,11 +33,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
+  <si>
+    <t xml:space="preserve">Accelerometer file name </t>
+  </si>
   <si>
     <t>Accelerometer model</t>
   </si>
   <si>
+    <t>Accelerometer wear location</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sex </t>
   </si>
   <si>
@@ -53,9 +59,42 @@
     <t>Waist circumference</t>
   </si>
   <si>
+    <t>SES</t>
+  </si>
+  <si>
+    <t>Maturational status</t>
+  </si>
+  <si>
+    <t>Ethnicity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sleep medications </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sleep conditions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country </t>
+  </si>
+  <si>
+    <t xml:space="preserve">City </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time Zone </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Season </t>
+  </si>
+  <si>
+    <t>The ID of the accelerometer file for each participant</t>
+  </si>
+  <si>
     <t>Please insert model of accelerometer. If different accelerometers have been used, please indicate (e.g. GT3X, wGT3X)</t>
   </si>
   <si>
+    <t>1: Wrist; 2: Hip; 3: Thigh (Please insert 1, 2, or 3)</t>
+  </si>
+  <si>
     <t>1: Female; 2: Male (Please insert 1 or 2)</t>
   </si>
   <si>
@@ -71,10 +110,157 @@
     <t>Waist circumference in cm (1 decimal place)</t>
   </si>
   <si>
-    <t>SES</t>
-  </si>
-  <si>
-    <t>Accelerometer wear location</t>
+    <r>
+      <t>Please indicate your SES scale using the mumerical codes in the SES sheet tab (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>insert 1-10 in column C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>If available, please indicate which maturational status measurement you have used (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>insert details in column C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>If available, please indicate how you have represented ethnicity (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>insert details in column C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>If available, please indicate how you have represented sleep medications (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>insert details in column C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>If available, please indicate diagnosed sleep conditions (insomnia, apnea, RLS etc.) and how these are represented (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>insert details in column C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+  </si>
+  <si>
+    <t>Country in which data were collected</t>
+  </si>
+  <si>
+    <t>City in which data were collected</t>
+  </si>
+  <si>
+    <r>
+      <t>Time zone where data were collected (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>insert details in column C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Season in which data were collected 1: Summer; 2: Winter </t>
   </si>
   <si>
     <t>Family wealth</t>
@@ -83,6 +269,9 @@
     <t xml:space="preserve">2-level scale </t>
   </si>
   <si>
+    <t>‘Better off’ or ‘poor’ based on basic needs being met (e.g. water, electricity).</t>
+  </si>
+  <si>
     <t>SIMD rank decile</t>
   </si>
   <si>
@@ -104,6 +293,9 @@
     <t xml:space="preserve">Mother education </t>
   </si>
   <si>
+    <t>1=10th grade or less, 2=vocational education, 3=high school education, 4=short tertiary education, 5=bachelor’s degree or equivalent, 6=master’s degree or higher.</t>
+  </si>
+  <si>
     <t>Parent education</t>
   </si>
   <si>
@@ -143,47 +335,11 @@
     <t xml:space="preserve">Other </t>
   </si>
   <si>
-    <t>1: Wrist; 2: Hip; 3: Thigh (Please insert 1, 2, or 3)</t>
-  </si>
-  <si>
-    <t>Maturational status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sleep medications </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sleep conditions </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country </t>
-  </si>
-  <si>
-    <t xml:space="preserve">City </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time Zone </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Season </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Season in which data were collected 1: Summer; 2: Winter </t>
-  </si>
-  <si>
-    <t>City in which data were collected</t>
-  </si>
-  <si>
-    <t>Country in which data were collected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accelerometer file name </t>
-  </si>
-  <si>
-    <t>The ID of the accelerometer file for each participant</t>
-  </si>
-  <si>
-    <r>
-      <t>Please indicate your SES scale using the mumerical codes in the SES sheet tab (</t>
+    <t xml:space="preserve">Screen time </t>
+  </si>
+  <si>
+    <r>
+      <t>If available, please indicate screen time (eg. discretionary or total screentime) (</t>
     </r>
     <r>
       <rPr>
@@ -193,30 +349,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>insert 1-10 in column C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>If available, please indicate which maturational status measurement you have used (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>insert details in column C</t>
     </r>
     <r>
@@ -228,111 +360,6 @@
       </rPr>
       <t xml:space="preserve">) </t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>If available, please indicate how you have represented ethnicity (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>insert details in column C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>If available, please indicate how you have represented sleep medications (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>insert details in column C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>If available, please indicate diagnosed sleep conditions (insomnia, apnea, RLS etc.) and how these are represented (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>insert details in column C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Time zone where data were collected (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>insert details in column C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-  </si>
-  <si>
-    <t>Ethnicity</t>
-  </si>
-  <si>
-    <t>Better off' or 'poor' based on basic needs being met (e.g. water, electricity).</t>
-  </si>
-  <si>
-    <t>1=10th grade or less, 2=vocational education, 3=high school education, 4=short tertiary education, 5=bachelor's degree or equivalent, 6=master's degree or higher.</t>
   </si>
 </sst>
 </file>
@@ -405,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -413,7 +440,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,10 +723,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -714,58 +740,64 @@
     <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>43</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -774,10 +806,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5EF2728-2369-450A-B5D5-1F6C65BB68AD}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -789,144 +821,153 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -940,7 +981,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -955,13 +996,13 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>56</v>
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -969,13 +1010,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -983,13 +1024,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -997,13 +1038,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1011,13 +1052,13 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1025,13 +1066,13 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1039,13 +1080,13 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1053,13 +1094,13 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1067,13 +1108,13 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1081,7 +1122,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>